<commit_message>
fix: upddated attribute sheet
</commit_message>
<xml_diff>
--- a/api/components/attributes/metro/metro_attributes_updated.xlsx
+++ b/api/components/attributes/metro/metro_attributes_updated.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4280" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4304" uniqueCount="443">
   <si>
     <t>Path</t>
   </si>
@@ -7008,7 +7008,44 @@
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="E102" s="77"/>
+      <c r="A102" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E102" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
+      <c r="M102" s="19"/>
+      <c r="N102" s="19"/>
+      <c r="O102" s="19"/>
+      <c r="P102" s="19"/>
+      <c r="Q102" s="19"/>
+      <c r="R102" s="19"/>
+      <c r="S102" s="19"/>
+      <c r="T102" s="19"/>
+      <c r="U102" s="19"/>
+      <c r="V102" s="19"/>
+      <c r="W102" s="19"/>
+      <c r="X102" s="19"/>
+      <c r="Y102" s="19"/>
+      <c r="Z102" s="19"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="E103" s="77"/>
@@ -14298,7 +14335,46 @@
       <c r="Y101" s="2"/>
       <c r="Z101" s="2"/>
     </row>
-    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1">
+      <c r="A102" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E102" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
+      <c r="M102" s="19"/>
+      <c r="N102" s="19"/>
+      <c r="O102" s="19"/>
+      <c r="P102" s="19"/>
+      <c r="Q102" s="19"/>
+      <c r="R102" s="19"/>
+      <c r="S102" s="19"/>
+      <c r="T102" s="19"/>
+      <c r="U102" s="19"/>
+      <c r="V102" s="19"/>
+      <c r="W102" s="19"/>
+      <c r="X102" s="19"/>
+      <c r="Y102" s="19"/>
+      <c r="Z102" s="19"/>
+    </row>
     <row r="103" ht="15.75" customHeight="1"/>
     <row r="104" ht="15.75" customHeight="1"/>
     <row r="105" ht="15.75" customHeight="1"/>
@@ -53131,7 +53207,46 @@
       <c r="Y94" s="2"/>
       <c r="Z94" s="2"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="A95" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C95" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E95" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="G95" s="19"/>
+      <c r="H95" s="19"/>
+      <c r="I95" s="19"/>
+      <c r="J95" s="19"/>
+      <c r="K95" s="19"/>
+      <c r="L95" s="19"/>
+      <c r="M95" s="19"/>
+      <c r="N95" s="19"/>
+      <c r="O95" s="19"/>
+      <c r="P95" s="19"/>
+      <c r="Q95" s="19"/>
+      <c r="R95" s="19"/>
+      <c r="S95" s="19"/>
+      <c r="T95" s="19"/>
+      <c r="U95" s="19"/>
+      <c r="V95" s="19"/>
+      <c r="W95" s="19"/>
+      <c r="X95" s="19"/>
+      <c r="Y95" s="19"/>
+      <c r="Z95" s="19"/>
+    </row>
     <row r="96" ht="15.75" customHeight="1"/>
     <row r="97" ht="15.75" customHeight="1"/>
     <row r="98" ht="15.75" customHeight="1"/>
@@ -59314,7 +59429,46 @@
       <c r="Y105" s="2"/>
       <c r="Z105" s="2"/>
     </row>
-    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1">
+      <c r="A106" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C106" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E106" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="G106" s="19"/>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="19"/>
+      <c r="L106" s="19"/>
+      <c r="M106" s="19"/>
+      <c r="N106" s="19"/>
+      <c r="O106" s="19"/>
+      <c r="P106" s="19"/>
+      <c r="Q106" s="19"/>
+      <c r="R106" s="19"/>
+      <c r="S106" s="19"/>
+      <c r="T106" s="19"/>
+      <c r="U106" s="19"/>
+      <c r="V106" s="19"/>
+      <c r="W106" s="19"/>
+      <c r="X106" s="19"/>
+      <c r="Y106" s="19"/>
+      <c r="Z106" s="19"/>
+    </row>
     <row r="107" ht="15.75" customHeight="1"/>
     <row r="108" ht="15.75" customHeight="1"/>
     <row r="109" ht="15.75" customHeight="1"/>

</xml_diff>